<commit_message>
feat: update excel reader
</commit_message>
<xml_diff>
--- a/src/excel/test/uart.xlsx
+++ b/src/excel/test/uart.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="10480"/>
+    <workbookView windowWidth="19200" windowHeight="14490"/>
   </bookViews>
   <sheets>
     <sheet name="uart" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="34">
   <si>
     <t>Module Inst Name</t>
   </si>
@@ -55,6 +55,9 @@
     <t>input</t>
   </si>
   <si>
+    <t>test reset</t>
+  </si>
+  <si>
     <t>m_axis_tready</t>
   </si>
   <si>
@@ -76,6 +79,9 @@
     <t>frame_error</t>
   </si>
   <si>
+    <t>has some error</t>
+  </si>
+  <si>
     <t>s_axis_tvalid</t>
   </si>
   <si>
@@ -100,6 +106,9 @@
     <t>rx_busy</t>
   </si>
   <si>
+    <t>may be error</t>
+  </si>
+  <si>
     <t>rx_overrun_error</t>
   </si>
   <si>
@@ -115,7 +124,13 @@
     <t>s_axis_tdata</t>
   </si>
   <si>
+    <t>一二三四五</t>
+  </si>
+  <si>
     <t>tx_busy</t>
+  </si>
+  <si>
+    <t>上山打老虎</t>
   </si>
 </sst>
 </file>
@@ -128,7 +143,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,13 +154,6 @@
     <font>
       <b/>
       <sz val="16"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -616,148 +624,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1120,15 +1128,15 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="30.7090909090909" customWidth="1"/>
-    <col min="2" max="3" width="10.7090909090909" customWidth="1"/>
-    <col min="4" max="4" width="30.7090909090909" customWidth="1"/>
-    <col min="5" max="5" width="40.7090909090909" customWidth="1"/>
+    <col min="1" max="1" width="30.7083333333333" customWidth="1"/>
+    <col min="2" max="3" width="10.7083333333333" customWidth="1"/>
+    <col min="4" max="4" width="30.7083333333333" customWidth="1"/>
+    <col min="5" max="5" width="40.7083333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="18" customHeight="1" spans="1:1">
@@ -1153,7 +1161,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" ht="16" customHeight="1" spans="1:3">
+    <row r="3" ht="16" customHeight="1" spans="1:5">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1163,10 +1171,13 @@
       <c r="C3" s="2">
         <v>1</v>
       </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" ht="16" customHeight="1" spans="1:3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -1177,7 +1188,7 @@
     </row>
     <row r="5" ht="16" customHeight="1" spans="1:3">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -1188,10 +1199,10 @@
     </row>
     <row r="6" ht="16" customHeight="1" spans="1:3">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
@@ -1199,7 +1210,7 @@
     </row>
     <row r="7" ht="16" customHeight="1" spans="1:3">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -1210,29 +1221,32 @@
     </row>
     <row r="8" ht="16" customHeight="1" spans="1:3">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C8" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="9" ht="16" customHeight="1" spans="1:3">
+    <row r="9" ht="16" customHeight="1" spans="1:5">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C9" s="2">
         <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="10" ht="16" customHeight="1" spans="1:3">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -1243,10 +1257,10 @@
     </row>
     <row r="11" ht="16" customHeight="1" spans="1:3">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C11" s="2">
         <v>1</v>
@@ -1254,7 +1268,7 @@
     </row>
     <row r="12" ht="16" customHeight="1" spans="1:3">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
@@ -1265,10 +1279,10 @@
     </row>
     <row r="13" ht="16" customHeight="1" spans="1:3">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C13" s="2">
         <v>1</v>
@@ -1276,10 +1290,10 @@
     </row>
     <row r="14" ht="16" customHeight="1" spans="1:3">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C14" s="2">
         <v>1</v>
@@ -1299,15 +1313,15 @@
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="30.7090909090909" customWidth="1"/>
-    <col min="2" max="3" width="10.7090909090909" customWidth="1"/>
-    <col min="4" max="4" width="30.7090909090909" customWidth="1"/>
-    <col min="5" max="5" width="40.7090909090909" customWidth="1"/>
+    <col min="1" max="1" width="30.7083333333333" customWidth="1"/>
+    <col min="2" max="3" width="10.7083333333333" customWidth="1"/>
+    <col min="4" max="4" width="30.7083333333333" customWidth="1"/>
+    <col min="5" max="5" width="40.7083333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="18" customHeight="1" spans="1:2">
@@ -1315,7 +1329,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" ht="20" customHeight="1" spans="1:5">
@@ -1337,7 +1351,7 @@
     </row>
     <row r="3" ht="16" customHeight="1" spans="1:4">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -1346,7 +1360,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" ht="16" customHeight="1" spans="1:4">
@@ -1365,35 +1379,35 @@
     </row>
     <row r="5" ht="16" customHeight="1" spans="1:4">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" s="2">
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" ht="16" customHeight="1" spans="1:4">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" ht="16" customHeight="1" spans="1:4">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -1402,12 +1416,12 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" ht="16" customHeight="1" spans="1:4">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -1416,54 +1430,57 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" ht="16" customHeight="1" spans="1:4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" ht="16" customHeight="1" spans="1:5">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C9" s="2">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>24</v>
+      </c>
+      <c r="E9" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="10" ht="16" customHeight="1" spans="1:4">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C10" s="2">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" ht="16" customHeight="1" spans="1:4">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C11" s="2">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" ht="16" customHeight="1" spans="1:4">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
@@ -1472,7 +1489,7 @@
         <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1489,15 +1506,15 @@
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+      <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="30.7090909090909" customWidth="1"/>
-    <col min="2" max="3" width="10.7090909090909" customWidth="1"/>
-    <col min="4" max="4" width="30.7090909090909" customWidth="1"/>
-    <col min="5" max="5" width="40.7090909090909" customWidth="1"/>
+    <col min="1" max="1" width="30.7083333333333" customWidth="1"/>
+    <col min="2" max="3" width="10.7083333333333" customWidth="1"/>
+    <col min="4" max="4" width="30.7083333333333" customWidth="1"/>
+    <col min="5" max="5" width="40.7083333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="18" customHeight="1" spans="1:2">
@@ -1505,7 +1522,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" ht="20" customHeight="1" spans="1:5">
@@ -1527,7 +1544,7 @@
     </row>
     <row r="3" ht="16" customHeight="1" spans="1:4">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -1536,7 +1553,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" ht="16" customHeight="1" spans="1:4">
@@ -1555,7 +1572,7 @@
     </row>
     <row r="5" ht="16" customHeight="1" spans="1:4">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -1564,12 +1581,12 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" ht="16" customHeight="1" spans="1:4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" ht="16" customHeight="1" spans="1:5">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -1578,54 +1595,57 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="7" ht="16" customHeight="1" spans="1:4">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C7" s="2">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" ht="16" customHeight="1" spans="1:4">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
         <v>11</v>
-      </c>
-      <c r="C8" s="2">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="9" ht="16" customHeight="1" spans="1:4">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C9" s="2">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" ht="16" customHeight="1" spans="1:4">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" ht="16" customHeight="1" spans="1:5">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -1634,7 +1654,10 @@
         <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>28</v>
+      </c>
+      <c r="E10" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add `generate_or_update` function in excel_writer
</commit_message>
<xml_diff>
--- a/src/excel/test/uart.xlsx
+++ b/src/excel/test/uart.xlsx
@@ -1,22 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView windowWidth="19200" windowHeight="14490" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="uart" sheetId="1" r:id="rId1"/>
     <sheet name="uart_rx" sheetId="2" r:id="rId2"/>
     <sheet name="uart_tx" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="30">
   <si>
     <t>Module Inst Name</t>
   </si>
@@ -57,6 +70,9 @@
     <t>m_axis_tvalid</t>
   </si>
   <si>
+    <t>safasdf</t>
+  </si>
+  <si>
     <t>overrun_error</t>
   </si>
   <si>
@@ -84,6 +100,15 @@
     <t>m_axis_tdata</t>
   </si>
   <si>
+    <t>rx_busy</t>
+  </si>
+  <si>
+    <t>rx_overrun_error</t>
+  </si>
+  <si>
+    <t>rx_frame_error</t>
+  </si>
+  <si>
     <t>prescale[15:0]</t>
   </si>
   <si>
@@ -91,38 +116,198 @@
   </si>
   <si>
     <t>s_axis_tdata</t>
+  </si>
+  <si>
+    <t>tx_busy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -135,8 +320,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -155,9 +526,251 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -171,11 +784,63 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -458,33 +1123,34 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="2" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" customWidth="1"/>
+    <col min="1" max="1" width="30.7083333333333" customWidth="1"/>
+    <col min="2" max="3" width="10.7083333333333" customWidth="1"/>
+    <col min="4" max="4" width="30.7083333333333" customWidth="1"/>
+    <col min="5" max="5" width="40.7083333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" customHeight="1">
+    <row r="1" ht="18" customHeight="1" spans="1:1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="20" customHeight="1">
+    <row r="2" ht="20" customHeight="1" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -501,7 +1167,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16" customHeight="1">
+    <row r="3" ht="16" customHeight="1" spans="1:3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -512,7 +1178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16" customHeight="1">
+    <row r="4" ht="16" customHeight="1" spans="1:3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -523,7 +1189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="16" customHeight="1">
+    <row r="5" ht="16" customHeight="1" spans="1:3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -534,7 +1200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16" customHeight="1">
+    <row r="6" ht="16" customHeight="1" spans="1:3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -545,7 +1211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16" customHeight="1">
+    <row r="7" ht="16" customHeight="1" spans="1:5">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -555,10 +1221,13 @@
       <c r="C7" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="16" customHeight="1">
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" ht="16" customHeight="1" spans="1:3">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -567,9 +1236,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="16" customHeight="1">
+    <row r="9" ht="16" customHeight="1" spans="1:3">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
@@ -578,9 +1247,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="16" customHeight="1">
+    <row r="10" ht="16" customHeight="1" spans="1:3">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
@@ -589,9 +1258,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="16" customHeight="1">
+    <row r="11" ht="16" customHeight="1" spans="1:3">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
@@ -600,9 +1269,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="16" customHeight="1">
+    <row r="12" ht="16" customHeight="1" spans="1:3">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
@@ -611,9 +1280,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="16" customHeight="1">
+    <row r="13" ht="16" customHeight="1" spans="1:3">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
         <v>9</v>
@@ -622,9 +1291,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="16" customHeight="1">
+    <row r="14" ht="16" customHeight="1" spans="1:3">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
@@ -635,35 +1304,38 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="2" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" customWidth="1"/>
+    <col min="1" max="1" width="30.7083333333333" customWidth="1"/>
+    <col min="2" max="3" width="10.7083333333333" customWidth="1"/>
+    <col min="4" max="4" width="30.7083333333333" customWidth="1"/>
+    <col min="5" max="5" width="40.7083333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" customHeight="1">
+    <row r="1" ht="18" customHeight="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="20" customHeight="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" ht="20" customHeight="1" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -680,7 +1352,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16" customHeight="1">
+    <row r="3" ht="16" customHeight="1" spans="1:4">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -694,9 +1366,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16" customHeight="1">
+    <row r="4" ht="16" customHeight="1" spans="1:4">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -705,12 +1377,12 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="16" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" ht="16" customHeight="1" spans="1:4">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -719,10 +1391,10 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="16" customHeight="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" ht="16" customHeight="1" spans="1:4">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -736,7 +1408,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16" customHeight="1">
+    <row r="7" ht="16" customHeight="1" spans="1:4">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -750,9 +1422,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="16" customHeight="1">
+    <row r="8" ht="16" customHeight="1" spans="1:5">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -761,10 +1433,13 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="16" customHeight="1">
+        <v>17</v>
+      </c>
+      <c r="E8">
+        <v>123123</v>
+      </c>
+    </row>
+    <row r="9" ht="16" customHeight="1" spans="1:4">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -775,12 +1450,12 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="16" customHeight="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" ht="16" customHeight="1" spans="1:4">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -789,10 +1464,10 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="16" customHeight="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" ht="16" customHeight="1" spans="1:4">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -803,12 +1478,12 @@
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="16" customHeight="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" ht="16" customHeight="1" spans="1:4">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
@@ -817,40 +1492,43 @@
         <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="2" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" customWidth="1"/>
+    <col min="1" max="1" width="30.7083333333333" customWidth="1"/>
+    <col min="2" max="3" width="10.7083333333333" customWidth="1"/>
+    <col min="4" max="4" width="30.7083333333333" customWidth="1"/>
+    <col min="5" max="5" width="40.7083333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" customHeight="1">
+    <row r="1" ht="18" customHeight="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="20" customHeight="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" ht="20" customHeight="1" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -867,7 +1545,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16" customHeight="1">
+    <row r="3" ht="16" customHeight="1" spans="1:4">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -881,9 +1559,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16" customHeight="1">
+    <row r="4" ht="16" customHeight="1" spans="1:4">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -892,12 +1570,12 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="16" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" ht="16" customHeight="1" spans="1:5">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
@@ -906,12 +1584,15 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="16" customHeight="1">
+        <v>28</v>
+      </c>
+      <c r="E5">
+        <v>5465</v>
+      </c>
+    </row>
+    <row r="6" ht="16" customHeight="1" spans="1:4">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
@@ -920,12 +1601,12 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" ht="16" customHeight="1" spans="1:4">
+      <c r="A7" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="16" customHeight="1">
-      <c r="A7" t="s">
-        <v>17</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -934,12 +1615,12 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="16" customHeight="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" ht="16" customHeight="1" spans="1:4">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -948,10 +1629,10 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="16" customHeight="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" ht="16" customHeight="1" spans="1:4">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -962,12 +1643,12 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="16" customHeight="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" ht="16" customHeight="1" spans="1:4">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
@@ -976,10 +1657,11 @@
         <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: fix bug of WireBuilder dead lock
</commit_message>
<xml_diff>
--- a/src/excel/test/uart.xlsx
+++ b/src/excel/test/uart.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="34">
   <si>
     <t>Module Inst Name</t>
   </si>
@@ -51,12 +51,30 @@
     <t>output</t>
   </si>
   <si>
+    <t>fsdf</t>
+  </si>
+  <si>
     <t>prescale</t>
   </si>
   <si>
     <t>rst</t>
   </si>
   <si>
+    <t>sfdf</t>
+  </si>
+  <si>
+    <t>rxd</t>
+  </si>
+  <si>
+    <t>s_axis_tready</t>
+  </si>
+  <si>
+    <t>s_axis_tvalid</t>
+  </si>
+  <si>
+    <t>txd</t>
+  </si>
+  <si>
     <t>rx_busy</t>
   </si>
   <si>
@@ -66,28 +84,16 @@
     <t>rx_overrun_error</t>
   </si>
   <si>
-    <t>rxd</t>
-  </si>
-  <si>
-    <t>s_axis_tready</t>
-  </si>
-  <si>
-    <t>s_axis_tvalid</t>
-  </si>
-  <si>
     <t>tx_busy</t>
   </si>
   <si>
-    <t>txd</t>
-  </si>
-  <si>
     <t>u_uart_rx</t>
   </si>
   <si>
     <t>m_axis_tdata</t>
   </si>
   <si>
-    <t>sdfsdf</t>
+    <t>sdf</t>
   </si>
   <si>
     <t>busy</t>
@@ -105,7 +111,13 @@
     <t>u_uart_tx</t>
   </si>
   <si>
+    <t>ert</t>
+  </si>
+  <si>
     <t>s_axis_tdata</t>
+  </si>
+  <si>
+    <t>dfg</t>
   </si>
 </sst>
 </file>
@@ -548,10 +560,13 @@
       <c r="C5" s="3">
         <v>1</v>
       </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="6" spans="1:5" ht="16" customHeight="1">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -562,21 +577,24 @@
     </row>
     <row r="7" spans="1:5" ht="16" customHeight="1">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="3">
         <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16" customHeight="1">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C8" s="3">
         <v>1</v>
@@ -584,21 +602,24 @@
     </row>
     <row r="9" spans="1:5" ht="16" customHeight="1">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="3">
         <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="16" customHeight="1">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C10" s="3">
         <v>1</v>
@@ -606,10 +627,10 @@
     </row>
     <row r="11" spans="1:5" ht="16" customHeight="1">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C11" s="3">
         <v>1</v>
@@ -617,7 +638,7 @@
     </row>
     <row r="12" spans="1:5" ht="16" customHeight="1">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
@@ -628,10 +649,10 @@
     </row>
     <row r="13" spans="1:5" ht="16" customHeight="1">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C13" s="3">
         <v>1</v>
@@ -639,7 +660,7 @@
     </row>
     <row r="14" spans="1:5" ht="16" customHeight="1">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
@@ -650,7 +671,7 @@
     </row>
     <row r="15" spans="1:5" ht="16" customHeight="1">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
@@ -686,7 +707,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="20" customHeight="1">
@@ -722,7 +743,7 @@
     </row>
     <row r="4" spans="1:5" ht="16" customHeight="1">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -731,12 +752,12 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="16" customHeight="1">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -745,7 +766,10 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16" customHeight="1">
@@ -778,7 +802,7 @@
     </row>
     <row r="8" spans="1:5" ht="16" customHeight="1">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -787,15 +811,12 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="16" customHeight="1">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -804,12 +825,12 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="16" customHeight="1">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -818,12 +839,15 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>21</v>
+      </c>
+      <c r="E10" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="16" customHeight="1">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -832,12 +856,12 @@
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="16" customHeight="1">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
@@ -846,7 +870,7 @@
         <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -876,7 +900,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="20" customHeight="1">
@@ -912,7 +936,7 @@
     </row>
     <row r="4" spans="1:5" ht="16" customHeight="1">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -921,12 +945,15 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="16" customHeight="1">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -935,15 +962,12 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16" customHeight="1">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -952,12 +976,12 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16" customHeight="1">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -966,12 +990,15 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="E7" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16" customHeight="1">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -980,12 +1007,12 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="16" customHeight="1">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -994,12 +1021,12 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="16" customHeight="1">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -1008,7 +1035,7 @@
         <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: fix bug of WireBuilder lock
</commit_message>
<xml_diff>
--- a/src/excel/test/uart.xlsx
+++ b/src/excel/test/uart.xlsx
@@ -1,17 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView windowWidth="19200" windowHeight="14460" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="uart" sheetId="1" r:id="rId1"/>
     <sheet name="uart_rx" sheetId="2" r:id="rId2"/>
     <sheet name="uart_tx" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -123,33 +136,190 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -162,8 +332,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -182,9 +538,251 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -198,11 +796,63 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -485,33 +1135,34 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="2" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" customWidth="1"/>
+    <col min="1" max="1" width="30.7083333333333" customWidth="1"/>
+    <col min="2" max="3" width="10.7083333333333" customWidth="1"/>
+    <col min="4" max="4" width="30.7083333333333" customWidth="1"/>
+    <col min="5" max="5" width="40.7083333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" customHeight="1">
+    <row r="1" ht="18" customHeight="1" spans="1:1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="20" customHeight="1">
+    <row r="2" ht="20" customHeight="1" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -528,7 +1179,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16" customHeight="1">
+    <row r="3" ht="16" customHeight="1" spans="1:3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -539,7 +1190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16" customHeight="1">
+    <row r="4" ht="16" customHeight="1" spans="1:3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -550,7 +1201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="16" customHeight="1">
+    <row r="5" ht="16" customHeight="1" spans="1:5">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -564,7 +1215,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16" customHeight="1">
+    <row r="6" ht="16" customHeight="1" spans="1:3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -575,7 +1226,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16" customHeight="1">
+    <row r="7" ht="16" customHeight="1" spans="1:5">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -589,7 +1240,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="16" customHeight="1">
+    <row r="8" ht="16" customHeight="1" spans="1:3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -600,7 +1251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="16" customHeight="1">
+    <row r="9" ht="16" customHeight="1" spans="1:5">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -614,7 +1265,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="16" customHeight="1">
+    <row r="10" ht="16" customHeight="1" spans="1:3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -625,7 +1276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="16" customHeight="1">
+    <row r="11" ht="16" customHeight="1" spans="1:3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -636,7 +1287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="16" customHeight="1">
+    <row r="12" ht="16" customHeight="1" spans="1:3">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -647,7 +1298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="16" customHeight="1">
+    <row r="13" ht="16" customHeight="1" spans="1:3">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -658,7 +1309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="16" customHeight="1">
+    <row r="14" ht="16" customHeight="1" spans="1:3">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -669,7 +1320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="16" customHeight="1">
+    <row r="15" ht="16" customHeight="1" spans="1:3">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -682,27 +1333,30 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="2" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" customWidth="1"/>
+    <col min="1" max="1" width="30.7083333333333" customWidth="1"/>
+    <col min="2" max="3" width="10.7083333333333" customWidth="1"/>
+    <col min="4" max="4" width="30.7083333333333" customWidth="1"/>
+    <col min="5" max="5" width="40.7083333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" customHeight="1">
+    <row r="1" ht="18" customHeight="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -710,7 +1364,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="20" customHeight="1">
+    <row r="2" ht="20" customHeight="1" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -727,7 +1381,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16" customHeight="1">
+    <row r="3" ht="16" customHeight="1" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -741,7 +1395,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16" customHeight="1">
+    <row r="4" ht="16" customHeight="1" spans="1:4">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -755,7 +1409,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="16" customHeight="1">
+    <row r="5" ht="16" customHeight="1" spans="1:5">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -763,7 +1417,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" t="s">
         <v>24</v>
@@ -772,7 +1426,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16" customHeight="1">
+    <row r="6" ht="16" customHeight="1" spans="1:4">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -786,7 +1440,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16" customHeight="1">
+    <row r="7" ht="16" customHeight="1" spans="1:4">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -800,7 +1454,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="16" customHeight="1">
+    <row r="8" ht="16" customHeight="1" spans="1:4">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -814,7 +1468,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="16" customHeight="1">
+    <row r="9" ht="16" customHeight="1" spans="1:4">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -828,7 +1482,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="16" customHeight="1">
+    <row r="10" ht="16" customHeight="1" spans="1:5">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -845,7 +1499,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="16" customHeight="1">
+    <row r="11" ht="16" customHeight="1" spans="1:4">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -859,7 +1513,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="16" customHeight="1">
+    <row r="12" ht="16" customHeight="1" spans="1:4">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -875,27 +1529,30 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="2" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" customWidth="1"/>
+    <col min="1" max="1" width="30.7083333333333" customWidth="1"/>
+    <col min="2" max="3" width="10.7083333333333" customWidth="1"/>
+    <col min="4" max="4" width="30.7083333333333" customWidth="1"/>
+    <col min="5" max="5" width="40.7083333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" customHeight="1">
+    <row r="1" ht="18" customHeight="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -903,7 +1560,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="20" customHeight="1">
+    <row r="2" ht="20" customHeight="1" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -920,7 +1577,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16" customHeight="1">
+    <row r="3" ht="16" customHeight="1" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -934,7 +1591,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16" customHeight="1">
+    <row r="4" ht="16" customHeight="1" spans="1:5">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -951,7 +1608,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="16" customHeight="1">
+    <row r="5" ht="16" customHeight="1" spans="1:4">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -959,13 +1616,13 @@
         <v>7</v>
       </c>
       <c r="C5" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16" customHeight="1">
+    <row r="6" ht="16" customHeight="1" spans="1:4">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -979,7 +1636,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16" customHeight="1">
+    <row r="7" ht="16" customHeight="1" spans="1:5">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -996,7 +1653,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="16" customHeight="1">
+    <row r="8" ht="16" customHeight="1" spans="1:4">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1010,7 +1667,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="16" customHeight="1">
+    <row r="9" ht="16" customHeight="1" spans="1:4">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1024,7 +1681,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="16" customHeight="1">
+    <row r="10" ht="16" customHeight="1" spans="1:4">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1040,5 +1697,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: add debug message
</commit_message>
<xml_diff>
--- a/src/excel/test/uart.xlsx
+++ b/src/excel/test/uart.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="36">
   <si>
     <t>Module Inst Name</t>
   </si>
@@ -36,52 +36,79 @@
     <t>Port-info</t>
   </si>
   <si>
+    <t>clk</t>
+  </si>
+  <si>
+    <t>input</t>
+  </si>
+  <si>
+    <t>m_axis_tready</t>
+  </si>
+  <si>
+    <t>m_axis_tvalid</t>
+  </si>
+  <si>
+    <t>output</t>
+  </si>
+  <si>
+    <t>prescale</t>
+  </si>
+  <si>
+    <t>sfdaf</t>
+  </si>
+  <si>
+    <t>rst</t>
+  </si>
+  <si>
+    <t>rxd</t>
+  </si>
+  <si>
+    <t>s_axis_tready</t>
+  </si>
+  <si>
+    <t>sdfdf</t>
+  </si>
+  <si>
+    <t>s_axis_tvalid</t>
+  </si>
+  <si>
+    <t>txd</t>
+  </si>
+  <si>
+    <t>rx_busy</t>
+  </si>
+  <si>
+    <t>rx_frame_error</t>
+  </si>
+  <si>
+    <t>rx_overrun_error</t>
+  </si>
+  <si>
+    <t>tx_busy</t>
+  </si>
+  <si>
+    <t>u_uart_rx</t>
+  </si>
+  <si>
+    <t>tyur</t>
+  </si>
+  <si>
+    <t>m_axis_tdata</t>
+  </si>
+  <si>
+    <t>gfh</t>
+  </si>
+  <si>
     <t>busy</t>
   </si>
   <si>
-    <t>output</t>
-  </si>
-  <si>
-    <t>clk</t>
-  </si>
-  <si>
-    <t>input</t>
+    <t>overrun_error</t>
   </si>
   <si>
     <t>frame_error</t>
   </si>
   <si>
-    <t>m_axis_tready</t>
-  </si>
-  <si>
-    <t>m_axis_tvalid</t>
-  </si>
-  <si>
-    <t>overrun_error</t>
-  </si>
-  <si>
-    <t>prescale</t>
-  </si>
-  <si>
-    <t>rst</t>
-  </si>
-  <si>
-    <t>rxd</t>
-  </si>
-  <si>
-    <t>s_axis_tready</t>
-  </si>
-  <si>
-    <t>s_axis_tvalid</t>
-  </si>
-  <si>
-    <t>txd</t>
-  </si>
-  <si>
-    <t>u_uart_rx</t>
-  </si>
-  <si>
-    <t>m_axis_tdata</t>
+    <t>hdgfh</t>
   </si>
   <si>
     <t>prescale[15:0]</t>
@@ -90,7 +117,13 @@
     <t>u_uart_tx</t>
   </si>
   <si>
+    <t>sdfgfsdg</t>
+  </si>
+  <si>
     <t>s_axis_tdata</t>
+  </si>
+  <si>
+    <t>sfg</t>
   </si>
 </sst>
 </file>
@@ -464,7 +497,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -517,7 +550,7 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C4" s="3">
         <v>1</v>
@@ -525,10 +558,10 @@
     </row>
     <row r="5" spans="1:5" ht="16" customHeight="1">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C5" s="3">
         <v>1</v>
@@ -539,15 +572,18 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C6" s="3">
-        <v>1</v>
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16" customHeight="1">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -558,7 +594,7 @@
     </row>
     <row r="8" spans="1:5" ht="16" customHeight="1">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -569,21 +605,24 @@
     </row>
     <row r="9" spans="1:5" ht="16" customHeight="1">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C9" s="3">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="16" customHeight="1">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C10" s="3">
         <v>1</v>
@@ -591,10 +630,10 @@
     </row>
     <row r="11" spans="1:5" ht="16" customHeight="1">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C11" s="3">
         <v>1</v>
@@ -602,10 +641,10 @@
     </row>
     <row r="12" spans="1:5" ht="16" customHeight="1">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C12" s="3">
         <v>1</v>
@@ -613,10 +652,10 @@
     </row>
     <row r="13" spans="1:5" ht="16" customHeight="1">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C13" s="3">
         <v>1</v>
@@ -624,12 +663,23 @@
     </row>
     <row r="14" spans="1:5" ht="16" customHeight="1">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C14" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="16" customHeight="1">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="3">
         <v>1</v>
       </c>
     </row>
@@ -660,7 +710,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="20" customHeight="1">
@@ -682,142 +732,151 @@
     </row>
     <row r="3" spans="1:5" ht="16" customHeight="1">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" s="3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="16" customHeight="1">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C4" s="3">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="16" customHeight="1">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C5" s="3">
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16" customHeight="1">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C6" s="3">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16" customHeight="1">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C7" s="3">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16" customHeight="1">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C8" s="3">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="16" customHeight="1">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C9" s="3">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="16" customHeight="1">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C10" s="3">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="16" customHeight="1">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C11" s="3">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>20</v>
+      </c>
+      <c r="E11" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="16" customHeight="1">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C12" s="3">
         <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -847,7 +906,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="20" customHeight="1">
@@ -869,114 +928,120 @@
     </row>
     <row r="3" spans="1:5" ht="16" customHeight="1">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" s="3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="16" customHeight="1">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C4" s="3">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="16" customHeight="1">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C5" s="3">
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16" customHeight="1">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C6" s="3">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16" customHeight="1">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C7" s="3">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16" customHeight="1">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C8" s="3">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="16" customHeight="1">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C9" s="3">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>22</v>
+      </c>
+      <c r="E9" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="16" customHeight="1">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C10" s="3">
         <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: fix bug of output log
</commit_message>
<xml_diff>
--- a/src/excel/test/uart.xlsx
+++ b/src/excel/test/uart.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="32">
   <si>
     <t>Module Inst Name</t>
   </si>
@@ -33,7 +33,7 @@
     <t>Wire-name</t>
   </si>
   <si>
-    <t>Port-info</t>
+    <t>Port-comment</t>
   </si>
   <si>
     <t>clk</t>
@@ -54,9 +54,6 @@
     <t>prescale</t>
   </si>
   <si>
-    <t>sfdaf</t>
-  </si>
-  <si>
     <t>rst</t>
   </si>
   <si>
@@ -66,9 +63,6 @@
     <t>s_axis_tready</t>
   </si>
   <si>
-    <t>sdfdf</t>
-  </si>
-  <si>
     <t>s_axis_tvalid</t>
   </si>
   <si>
@@ -90,15 +84,9 @@
     <t>u_uart_rx</t>
   </si>
   <si>
-    <t>tyur</t>
-  </si>
-  <si>
     <t>m_axis_tdata</t>
   </si>
   <si>
-    <t>gfh</t>
-  </si>
-  <si>
     <t>busy</t>
   </si>
   <si>
@@ -108,22 +96,22 @@
     <t>frame_error</t>
   </si>
   <si>
-    <t>hdgfh</t>
-  </si>
-  <si>
     <t>prescale[15:0]</t>
   </si>
   <si>
     <t>u_uart_tx</t>
   </si>
   <si>
-    <t>sdfgfsdg</t>
-  </si>
-  <si>
     <t>s_axis_tdata</t>
   </si>
   <si>
-    <t>sfg</t>
+    <t>dsaf</t>
+  </si>
+  <si>
+    <t>asf</t>
+  </si>
+  <si>
+    <t>fdasf</t>
   </si>
 </sst>
 </file>
@@ -577,13 +565,10 @@
       <c r="C6" s="3">
         <v>16</v>
       </c>
-      <c r="E6" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="7" spans="1:5" ht="16" customHeight="1">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -594,7 +579,7 @@
     </row>
     <row r="8" spans="1:5" ht="16" customHeight="1">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -605,21 +590,18 @@
     </row>
     <row r="9" spans="1:5" ht="16" customHeight="1">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="3">
         <v>1</v>
-      </c>
-      <c r="E9" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="16" customHeight="1">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -630,7 +612,7 @@
     </row>
     <row r="11" spans="1:5" ht="16" customHeight="1">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -641,7 +623,7 @@
     </row>
     <row r="12" spans="1:5" ht="16" customHeight="1">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
@@ -652,7 +634,7 @@
     </row>
     <row r="13" spans="1:5" ht="16" customHeight="1">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -663,7 +645,7 @@
     </row>
     <row r="14" spans="1:5" ht="16" customHeight="1">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
@@ -674,7 +656,7 @@
     </row>
     <row r="15" spans="1:5" ht="16" customHeight="1">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
@@ -710,7 +692,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="20" customHeight="1">
@@ -746,7 +728,7 @@
     </row>
     <row r="4" spans="1:5" ht="16" customHeight="1">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -755,15 +737,12 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="16" customHeight="1">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -772,7 +751,7 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16" customHeight="1">
@@ -802,13 +781,10 @@
       <c r="D7" t="s">
         <v>8</v>
       </c>
-      <c r="E7" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="8" spans="1:5" ht="16" customHeight="1">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -817,12 +793,12 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="16" customHeight="1">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -831,12 +807,12 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="16" customHeight="1">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -845,12 +821,12 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="16" customHeight="1">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -859,10 +835,7 @@
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="16" customHeight="1">
@@ -876,7 +849,7 @@
         <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -906,7 +879,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="20" customHeight="1">
@@ -942,7 +915,7 @@
     </row>
     <row r="4" spans="1:5" ht="16" customHeight="1">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -951,15 +924,12 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="16" customHeight="1">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -968,12 +938,15 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>28</v>
+      </c>
+      <c r="E5" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16" customHeight="1">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -982,12 +955,12 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16" customHeight="1">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -996,12 +969,15 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16" customHeight="1">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -1010,12 +986,12 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="16" customHeight="1">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -1024,10 +1000,7 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="16" customHeight="1">
@@ -1041,6 +1014,9 @@
         <v>16</v>
       </c>
       <c r="D10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: fix bug of main port wire direction
</commit_message>
<xml_diff>
--- a/src/excel/test/uart.xlsx
+++ b/src/excel/test/uart.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="34">
   <si>
     <t>Module Inst Name</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>tx_busy</t>
+  </si>
+  <si>
+    <t>test_temp</t>
+  </si>
+  <si>
+    <t>test_port</t>
   </si>
   <si>
     <t>u_uart_rx</t>
@@ -485,7 +491,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -663,6 +669,23 @@
       </c>
       <c r="C15" s="3">
         <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="16" customHeight="1">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="3">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -692,7 +715,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="20" customHeight="1">
@@ -742,7 +765,7 @@
     </row>
     <row r="5" spans="1:5" ht="16" customHeight="1">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -751,7 +774,7 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16" customHeight="1">
@@ -798,7 +821,7 @@
     </row>
     <row r="9" spans="1:5" ht="16" customHeight="1">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -812,7 +835,7 @@
     </row>
     <row r="10" spans="1:5" ht="16" customHeight="1">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -826,7 +849,7 @@
     </row>
     <row r="11" spans="1:5" ht="16" customHeight="1">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -849,7 +872,7 @@
         <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -879,7 +902,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="20" customHeight="1">
@@ -929,7 +952,7 @@
     </row>
     <row r="5" spans="1:5" ht="16" customHeight="1">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -938,10 +961,10 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16" customHeight="1">
@@ -972,7 +995,7 @@
         <v>14</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16" customHeight="1">
@@ -991,7 +1014,7 @@
     </row>
     <row r="9" spans="1:5" ht="16" customHeight="1">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -1014,10 +1037,10 @@
         <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E10" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: highlight wire name which same with port name
</commit_message>
<xml_diff>
--- a/src/excel/test/uart.xlsx
+++ b/src/excel/test/uart.xlsx
@@ -124,7 +124,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,6 +143,14 @@
     <font>
       <b/>
       <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -186,7 +194,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -197,6 +205,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -745,7 +754,7 @@
       <c r="C3" s="3">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -759,7 +768,7 @@
       <c r="C4" s="3">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -773,7 +782,7 @@
       <c r="C5" s="3">
         <v>0</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="4" t="s">
         <v>24</v>
       </c>
     </row>
@@ -787,7 +796,7 @@
       <c r="C6" s="3">
         <v>1</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -801,7 +810,7 @@
       <c r="C7" s="3">
         <v>1</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -815,7 +824,7 @@
       <c r="C8" s="3">
         <v>1</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="4" t="s">
         <v>13</v>
       </c>
     </row>
@@ -871,7 +880,7 @@
       <c r="C12" s="3">
         <v>16</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="4" t="s">
         <v>28</v>
       </c>
     </row>
@@ -932,7 +941,7 @@
       <c r="C3" s="3">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -946,7 +955,7 @@
       <c r="C4" s="3">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -960,7 +969,7 @@
       <c r="C5" s="3">
         <v>0</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E5" t="s">
@@ -977,7 +986,7 @@
       <c r="C6" s="3">
         <v>1</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="4" t="s">
         <v>15</v>
       </c>
     </row>
@@ -991,7 +1000,7 @@
       <c r="C7" s="3">
         <v>1</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E7" t="s">
@@ -1008,7 +1017,7 @@
       <c r="C8" s="3">
         <v>1</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1036,7 +1045,7 @@
       <c r="C10" s="3">
         <v>16</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="4" t="s">
         <v>28</v>
       </c>
       <c r="E10" t="s">

</xml_diff>

<commit_message>
feat: highlight excel update change message
</commit_message>
<xml_diff>
--- a/src/excel/test/uart.xlsx
+++ b/src/excel/test/uart.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="35">
   <si>
     <t>Module Inst Name</t>
   </si>
@@ -42,6 +42,9 @@
     <t>input</t>
   </si>
   <si>
+    <t>adsfasf</t>
+  </si>
+  <si>
     <t>m_axis_tready</t>
   </si>
   <si>
@@ -51,6 +54,9 @@
     <t>output</t>
   </si>
   <si>
+    <t>adsfa</t>
+  </si>
+  <si>
     <t>prescale</t>
   </si>
   <si>
@@ -60,6 +66,9 @@
     <t>rxd</t>
   </si>
   <si>
+    <t>safda</t>
+  </si>
+  <si>
     <t>s_axis_tready</t>
   </si>
   <si>
@@ -81,18 +90,18 @@
     <t>tx_busy</t>
   </si>
   <si>
-    <t>test_temp</t>
-  </si>
-  <si>
-    <t>test_port</t>
-  </si>
-  <si>
     <t>u_uart_rx</t>
   </si>
   <si>
     <t>m_axis_tdata</t>
   </si>
   <si>
+    <t>dsaf</t>
+  </si>
+  <si>
+    <t>fgds</t>
+  </si>
+  <si>
     <t>busy</t>
   </si>
   <si>
@@ -102,6 +111,9 @@
     <t>frame_error</t>
   </si>
   <si>
+    <t>asdf</t>
+  </si>
+  <si>
     <t>prescale[15:0]</t>
   </si>
   <si>
@@ -109,15 +121,6 @@
   </si>
   <si>
     <t>s_axis_tdata</t>
-  </si>
-  <si>
-    <t>dsaf</t>
-  </si>
-  <si>
-    <t>asf</t>
-  </si>
-  <si>
-    <t>fdasf</t>
   </si>
 </sst>
 </file>
@@ -500,7 +503,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -547,10 +550,13 @@
       <c r="C3" s="3">
         <v>1</v>
       </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="16" customHeight="1">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -561,18 +567,21 @@
     </row>
     <row r="5" spans="1:5" ht="16" customHeight="1">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="3">
         <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16" customHeight="1">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -583,7 +592,7 @@
     </row>
     <row r="7" spans="1:5" ht="16" customHeight="1">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -594,21 +603,24 @@
     </row>
     <row r="8" spans="1:5" ht="16" customHeight="1">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="3">
         <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="16" customHeight="1">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C9" s="3">
         <v>1</v>
@@ -616,7 +628,7 @@
     </row>
     <row r="10" spans="1:5" ht="16" customHeight="1">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -627,10 +639,10 @@
     </row>
     <row r="11" spans="1:5" ht="16" customHeight="1">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C11" s="3">
         <v>1</v>
@@ -638,10 +650,10 @@
     </row>
     <row r="12" spans="1:5" ht="16" customHeight="1">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12" s="3">
         <v>1</v>
@@ -649,10 +661,10 @@
     </row>
     <row r="13" spans="1:5" ht="16" customHeight="1">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C13" s="3">
         <v>1</v>
@@ -660,10 +672,10 @@
     </row>
     <row r="14" spans="1:5" ht="16" customHeight="1">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C14" s="3">
         <v>1</v>
@@ -671,30 +683,13 @@
     </row>
     <row r="15" spans="1:5" ht="16" customHeight="1">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C15" s="3">
         <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="16" customHeight="1">
-      <c r="A16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="3">
-        <v>1</v>
-      </c>
-      <c r="D16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -724,7 +719,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="20" customHeight="1">
@@ -760,7 +755,7 @@
     </row>
     <row r="4" spans="1:5" ht="16" customHeight="1">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -769,40 +764,43 @@
         <v>1</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="16" customHeight="1">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="3">
         <v>0</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16" customHeight="1">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="C6" s="3">
-        <v>1</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16" customHeight="1">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -811,12 +809,12 @@
         <v>1</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16" customHeight="1">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -825,54 +823,60 @@
         <v>1</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="16" customHeight="1">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C9" s="3">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="16" customHeight="1">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C10" s="3">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="16" customHeight="1">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C11" s="3">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>18</v>
+        <v>21</v>
+      </c>
+      <c r="E11" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="16" customHeight="1">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
@@ -881,7 +885,7 @@
         <v>16</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -911,7 +915,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="20" customHeight="1">
@@ -947,7 +951,7 @@
     </row>
     <row r="4" spans="1:5" ht="16" customHeight="1">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -956,12 +960,12 @@
         <v>1</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="16" customHeight="1">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -970,15 +974,12 @@
         <v>0</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16" customHeight="1">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -987,57 +988,54 @@
         <v>1</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16" customHeight="1">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7" s="3">
         <v>1</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16" customHeight="1">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C8" s="3">
         <v>1</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="16" customHeight="1">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C9" s="3">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="16" customHeight="1">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -1046,10 +1044,7 @@
         <v>16</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: update excel writer for parameter
</commit_message>
<xml_diff>
--- a/src/excel/test/uart.xlsx
+++ b/src/excel/test/uart.xlsx
@@ -16,11 +16,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="29">
   <si>
     <t>Module Inst Name</t>
   </si>
   <si>
+    <t>Parameter:</t>
+  </si>
+  <si>
     <t>Port-name</t>
   </si>
   <si>
@@ -36,13 +39,22 @@
     <t>Port-comment</t>
   </si>
   <si>
+    <t>busy</t>
+  </si>
+  <si>
+    <t>output</t>
+  </si>
+  <si>
     <t>clk</t>
   </si>
   <si>
     <t>input</t>
   </si>
   <si>
-    <t>adsfasf</t>
+    <t>frame_error</t>
+  </si>
+  <si>
+    <t>m_axis_tdata</t>
   </si>
   <si>
     <t>m_axis_tready</t>
@@ -51,10 +63,7 @@
     <t>m_axis_tvalid</t>
   </si>
   <si>
-    <t>output</t>
-  </si>
-  <si>
-    <t>adsfa</t>
+    <t>overrun_error</t>
   </si>
   <si>
     <t>prescale</t>
@@ -66,7 +75,7 @@
     <t>rxd</t>
   </si>
   <si>
-    <t>safda</t>
+    <t>s_axis_tdata</t>
   </si>
   <si>
     <t>s_axis_tready</t>
@@ -78,40 +87,13 @@
     <t>txd</t>
   </si>
   <si>
-    <t>rx_busy</t>
-  </si>
-  <si>
-    <t>rx_frame_error</t>
-  </si>
-  <si>
-    <t>rx_overrun_error</t>
-  </si>
-  <si>
-    <t>tx_busy</t>
-  </si>
-  <si>
     <t>u_uart_rx</t>
   </si>
   <si>
-    <t>m_axis_tdata</t>
-  </si>
-  <si>
-    <t>dsaf</t>
-  </si>
-  <si>
-    <t>fgds</t>
-  </si>
-  <si>
-    <t>busy</t>
-  </si>
-  <si>
-    <t>overrun_error</t>
-  </si>
-  <si>
-    <t>frame_error</t>
-  </si>
-  <si>
-    <t>asdf</t>
+    <t>DATA_WIDTH</t>
+  </si>
+  <si>
+    <t>m_axis_tdata[7:0]</t>
   </si>
   <si>
     <t>prescale[15:0]</t>
@@ -120,7 +102,7 @@
     <t>u_uart_tx</t>
   </si>
   <si>
-    <t>s_axis_tdata</t>
+    <t>s_axis_tdata[7:0]</t>
   </si>
 </sst>
 </file>
@@ -503,7 +485,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -524,42 +506,33 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="20" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="16" customHeight="1">
-      <c r="A3" t="s">
+      <c r="E3" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="16" customHeight="1">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" s="3">
         <v>1</v>
@@ -567,60 +540,54 @@
     </row>
     <row r="5" spans="1:5" ht="16" customHeight="1">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="3">
         <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16" customHeight="1">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C6" s="3">
-        <v>16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16" customHeight="1">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C7" s="3">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16" customHeight="1">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C8" s="3">
         <v>1</v>
-      </c>
-      <c r="E8" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="16" customHeight="1">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C9" s="3">
         <v>1</v>
@@ -628,10 +595,10 @@
     </row>
     <row r="10" spans="1:5" ht="16" customHeight="1">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C10" s="3">
         <v>1</v>
@@ -639,21 +606,21 @@
     </row>
     <row r="11" spans="1:5" ht="16" customHeight="1">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="3">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="16" customHeight="1">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="3">
         <v>1</v>
@@ -661,10 +628,10 @@
     </row>
     <row r="13" spans="1:5" ht="16" customHeight="1">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" s="3">
         <v>1</v>
@@ -672,23 +639,45 @@
     </row>
     <row r="14" spans="1:5" ht="16" customHeight="1">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C14" s="3">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="16" customHeight="1">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C15" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="16" customHeight="1">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="16" customHeight="1">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="3">
         <v>1</v>
       </c>
     </row>
@@ -699,10 +688,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
@@ -719,173 +708,177 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="20" customHeight="1">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="B3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="20" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="C3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="16" customHeight="1">
-      <c r="A3" t="s">
+      <c r="E4" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="16" customHeight="1">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="16" customHeight="1">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16" customHeight="1">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="3">
         <v>1</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16" customHeight="1">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C7" s="3">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16" customHeight="1">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C8" s="3">
         <v>1</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="16" customHeight="1">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="3">
         <v>1</v>
       </c>
-      <c r="D9" t="s">
-        <v>20</v>
+      <c r="D9" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="16" customHeight="1">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" s="3">
         <v>1</v>
       </c>
-      <c r="D10" t="s">
-        <v>22</v>
+      <c r="D10" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="16" customHeight="1">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C11" s="3">
         <v>1</v>
       </c>
-      <c r="D11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" t="s">
-        <v>31</v>
+      <c r="D11" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="16" customHeight="1">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C12" s="3">
+        <v>1</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="16" customHeight="1">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="16" customHeight="1">
+      <c r="A14" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>32</v>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="3">
+        <v>16</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -895,10 +888,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
@@ -915,136 +908,149 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="20" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="16" customHeight="1">
-      <c r="A3" t="s">
+      <c r="E4" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="16" customHeight="1">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="16" customHeight="1">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C5" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16" customHeight="1">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C6" s="3">
         <v>1</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16" customHeight="1">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="3">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16" customHeight="1">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="3">
         <v>1</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="16" customHeight="1">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C9" s="3">
         <v>1</v>
       </c>
-      <c r="D9" t="s">
-        <v>23</v>
+      <c r="D9" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="16" customHeight="1">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="16" customHeight="1">
+      <c r="A11" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="3">
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="16" customHeight="1">
+      <c r="A12" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>32</v>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="3">
+        <v>16</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: update excel writer update logic
</commit_message>
<xml_diff>
--- a/src/excel/test/uart.xlsx
+++ b/src/excel/test/uart.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="32">
   <si>
     <t>Module Inst Name</t>
   </si>
@@ -39,64 +39,73 @@
     <t>Port-comment</t>
   </si>
   <si>
+    <t>clk</t>
+  </si>
+  <si>
+    <t>input</t>
+  </si>
+  <si>
+    <t>m_axis_tdata</t>
+  </si>
+  <si>
+    <t>output</t>
+  </si>
+  <si>
+    <t>m_axis_tready</t>
+  </si>
+  <si>
+    <t>m_axis_tvalid</t>
+  </si>
+  <si>
+    <t>prescale</t>
+  </si>
+  <si>
+    <t>rst</t>
+  </si>
+  <si>
+    <t>rxd</t>
+  </si>
+  <si>
+    <t>s_axis_tdata</t>
+  </si>
+  <si>
+    <t>s_axis_tready</t>
+  </si>
+  <si>
+    <t>s_axis_tvalid</t>
+  </si>
+  <si>
+    <t>txd</t>
+  </si>
+  <si>
+    <t>rx_busy</t>
+  </si>
+  <si>
+    <t>rx_frame_error</t>
+  </si>
+  <si>
+    <t>rx_overrun_error</t>
+  </si>
+  <si>
+    <t>tx_busy</t>
+  </si>
+  <si>
+    <t>u_uart_rx</t>
+  </si>
+  <si>
     <t>busy</t>
   </si>
   <si>
-    <t>output</t>
-  </si>
-  <si>
-    <t>clk</t>
-  </si>
-  <si>
-    <t>input</t>
+    <t>overrun_error</t>
   </si>
   <si>
     <t>frame_error</t>
   </si>
   <si>
-    <t>m_axis_tdata</t>
-  </si>
-  <si>
-    <t>m_axis_tready</t>
-  </si>
-  <si>
-    <t>m_axis_tvalid</t>
-  </si>
-  <si>
-    <t>overrun_error</t>
-  </si>
-  <si>
-    <t>prescale</t>
-  </si>
-  <si>
-    <t>rst</t>
-  </si>
-  <si>
-    <t>rxd</t>
-  </si>
-  <si>
-    <t>s_axis_tdata</t>
-  </si>
-  <si>
-    <t>s_axis_tready</t>
-  </si>
-  <si>
-    <t>s_axis_tvalid</t>
-  </si>
-  <si>
-    <t>txd</t>
-  </si>
-  <si>
-    <t>u_uart_rx</t>
-  </si>
-  <si>
-    <t>DATA_WIDTH</t>
+    <t>prescale[15:0]</t>
   </si>
   <si>
     <t>m_axis_tdata[7:0]</t>
-  </si>
-  <si>
-    <t>prescale[15:0]</t>
   </si>
   <si>
     <t>u_uart_tx</t>
@@ -485,7 +494,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -546,7 +555,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="3">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16" customHeight="1">
@@ -565,10 +574,10 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C7" s="3">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16" customHeight="1">
@@ -576,10 +585,10 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C8" s="3">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="16" customHeight="1">
@@ -609,10 +618,10 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C11" s="3">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="16" customHeight="1">
@@ -631,7 +640,7 @@
         <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C13" s="3">
         <v>1</v>
@@ -645,7 +654,7 @@
         <v>10</v>
       </c>
       <c r="C14" s="3">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="16" customHeight="1">
@@ -653,7 +662,7 @@
         <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C15" s="3">
         <v>1</v>
@@ -675,9 +684,20 @@
         <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C17" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="16" customHeight="1">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="3">
         <v>1</v>
       </c>
     </row>
@@ -688,10 +708,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
@@ -708,7 +728,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="20" customHeight="1">
@@ -717,47 +737,53 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="2" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="16" customHeight="1">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="16" customHeight="1">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5" s="3">
         <v>1</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16" customHeight="1">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -766,26 +792,26 @@
         <v>1</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16" customHeight="1">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="3">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16" customHeight="1">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -794,12 +820,12 @@
         <v>1</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="16" customHeight="1">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -807,13 +833,13 @@
       <c r="C9" s="3">
         <v>1</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>13</v>
+      <c r="D9" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="16" customHeight="1">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -821,64 +847,50 @@
       <c r="C10" s="3">
         <v>1</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>18</v>
+      <c r="D10" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="16" customHeight="1">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C11" s="3">
         <v>1</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>7</v>
+      <c r="D11" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="16" customHeight="1">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="3">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="16" customHeight="1">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C13" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="16" customHeight="1">
-      <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="3">
-        <v>16</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -888,10 +900,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
@@ -908,7 +920,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="20" customHeight="1">
@@ -917,75 +929,81 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="2" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="16" customHeight="1">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="16" customHeight="1">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5" s="3">
         <v>1</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16" customHeight="1">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C6" s="3">
         <v>1</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16" customHeight="1">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="3">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16" customHeight="1">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -994,63 +1012,49 @@
         <v>1</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="16" customHeight="1">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C9" s="3">
         <v>1</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>20</v>
+      <c r="D9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="16" customHeight="1">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="3">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="16" customHeight="1">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="16" customHeight="1">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="3">
-        <v>16</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: fix bug of excel reader without parameter
</commit_message>
<xml_diff>
--- a/src/excel/test/uart.xlsx
+++ b/src/excel/test/uart.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="33">
   <si>
     <t>Module Inst Name</t>
   </si>
@@ -93,6 +93,12 @@
     <t>u_uart_rx</t>
   </si>
   <si>
+    <t>DATA_WIDTH</t>
+  </si>
+  <si>
+    <t>m_axis_tdata[7:0]</t>
+  </si>
+  <si>
     <t>busy</t>
   </si>
   <si>
@@ -103,9 +109,6 @@
   </si>
   <si>
     <t>prescale[15:0]</t>
-  </si>
-  <si>
-    <t>m_axis_tdata[7:0]</t>
   </si>
   <si>
     <t>u_uart_tx</t>
@@ -708,10 +711,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
@@ -737,39 +740,33 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="2" t="s">
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="16" customHeight="1">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="16" customHeight="1">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
@@ -778,77 +775,77 @@
         <v>1</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16" customHeight="1">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C6" s="3">
         <v>1</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16" customHeight="1">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C7" s="3">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16" customHeight="1">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C8" s="3">
         <v>1</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="16" customHeight="1">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C9" s="3">
         <v>1</v>
       </c>
-      <c r="D9" t="s">
-        <v>20</v>
+      <c r="D9" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="16" customHeight="1">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C10" s="3">
         <v>1</v>
       </c>
-      <c r="D10" t="s">
-        <v>22</v>
+      <c r="D10" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="16" customHeight="1">
@@ -862,35 +859,49 @@
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="16" customHeight="1">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C12" s="3">
-        <v>16</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>28</v>
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="16" customHeight="1">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="3">
-        <v>0</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>29</v>
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="16" customHeight="1">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="3">
+        <v>16</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -900,10 +911,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
@@ -920,7 +931,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="20" customHeight="1">
@@ -929,39 +940,33 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="2" t="s">
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="16" customHeight="1">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="16" customHeight="1">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
@@ -970,12 +975,12 @@
         <v>1</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16" customHeight="1">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
@@ -984,40 +989,40 @@
         <v>1</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16" customHeight="1">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C7" s="3">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16" customHeight="1">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C8" s="3">
         <v>1</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="16" customHeight="1">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -1025,36 +1030,50 @@
       <c r="C9" s="3">
         <v>1</v>
       </c>
-      <c r="D9" t="s">
-        <v>23</v>
+      <c r="D9" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="16" customHeight="1">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C10" s="3">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="16" customHeight="1">
       <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="16" customHeight="1">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="3">
         <v>16</v>
       </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="3">
-        <v>0</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>31</v>
+      <c r="D12" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add parameter display for generate_v
</commit_message>
<xml_diff>
--- a/src/excel/test/uart.xlsx
+++ b/src/excel/test/uart.xlsx
@@ -1,22 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView windowWidth="23040" windowHeight="10480"/>
   </bookViews>
   <sheets>
     <sheet name="uart" sheetId="1" r:id="rId1"/>
     <sheet name="uart_rx" sheetId="2" r:id="rId2"/>
     <sheet name="uart_tx" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="42">
   <si>
     <t>Module Inst Name</t>
   </si>
@@ -51,6 +64,9 @@
     <t>output</t>
   </si>
   <si>
+    <t>asfasf</t>
+  </si>
+  <si>
     <t>m_axis_tready</t>
   </si>
   <si>
@@ -78,12 +94,18 @@
     <t>txd</t>
   </si>
   <si>
+    <t>asdf</t>
+  </si>
+  <si>
     <t>rx_busy</t>
   </si>
   <si>
     <t>rx_frame_error</t>
   </si>
   <si>
+    <t>sadf</t>
+  </si>
+  <si>
     <t>rx_overrun_error</t>
   </si>
   <si>
@@ -96,6 +118,9 @@
     <t>DATA_WIDTH</t>
   </si>
   <si>
+    <t>asdfasd</t>
+  </si>
+  <si>
     <t>m_axis_tdata[7:0]</t>
   </si>
   <si>
@@ -105,56 +130,228 @@
     <t>overrun_error</t>
   </si>
   <si>
+    <t>fdasf</t>
+  </si>
+  <si>
     <t>frame_error</t>
   </si>
   <si>
     <t>prescale[15:0]</t>
   </si>
   <si>
+    <t>asf</t>
+  </si>
+  <si>
     <t>u_uart_tx</t>
   </si>
   <si>
     <t>s_axis_tdata[7:0]</t>
+  </si>
+  <si>
+    <t>反对敢死队风格Z</t>
+  </si>
+  <si>
+    <t>告诉对方给</t>
+  </si>
+  <si>
+    <t>fdgs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -167,8 +364,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -187,9 +570,251 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -204,11 +829,63 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -491,38 +1168,39 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="2" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" customWidth="1"/>
+    <col min="1" max="1" width="30.7090909090909" customWidth="1"/>
+    <col min="2" max="3" width="10.7090909090909" customWidth="1"/>
+    <col min="4" max="4" width="30.7090909090909" customWidth="1"/>
+    <col min="5" max="5" width="40.7090909090909" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" customHeight="1">
+    <row r="1" ht="18" customHeight="1" spans="1:1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="20" customHeight="1">
+    <row r="2" ht="20" customHeight="1" spans="1:1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" ht="21.75" spans="1:5">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -539,7 +1217,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16" customHeight="1">
+    <row r="4" ht="16" customHeight="1" spans="1:3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -550,7 +1228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="16" customHeight="1">
+    <row r="5" ht="16" customHeight="1" spans="1:5">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -560,10 +1238,13 @@
       <c r="C5" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="16" customHeight="1">
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" ht="16" customHeight="1" spans="1:3">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
@@ -572,9 +1253,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16" customHeight="1">
+    <row r="7" ht="16" customHeight="1" spans="1:3">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -583,9 +1264,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="16" customHeight="1">
+    <row r="8" ht="16" customHeight="1" spans="1:3">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -594,9 +1275,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="16" customHeight="1">
+    <row r="9" ht="16" customHeight="1" spans="1:3">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
@@ -605,9 +1286,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="16" customHeight="1">
+    <row r="10" ht="16" customHeight="1" spans="1:3">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
@@ -616,9 +1297,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="16" customHeight="1">
+    <row r="11" ht="16" customHeight="1" spans="1:3">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
@@ -627,9 +1308,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="16" customHeight="1">
+    <row r="12" ht="16" customHeight="1" spans="1:3">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
@@ -638,9 +1319,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="16" customHeight="1">
+    <row r="13" ht="16" customHeight="1" spans="1:3">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
         <v>8</v>
@@ -649,9 +1330,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="16" customHeight="1">
+    <row r="14" ht="16" customHeight="1" spans="1:5">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
@@ -659,10 +1340,13 @@
       <c r="C14" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="16" customHeight="1">
+      <c r="E14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" ht="16" customHeight="1" spans="1:3">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
@@ -671,9 +1355,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="16" customHeight="1">
+    <row r="16" ht="16" customHeight="1" spans="1:5">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
@@ -681,10 +1365,13 @@
       <c r="C16" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="16" customHeight="1">
+      <c r="E16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" ht="16" customHeight="1" spans="1:3">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
@@ -693,9 +1380,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="16" customHeight="1">
+    <row r="18" ht="16" customHeight="1" spans="1:3">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
@@ -706,48 +1393,51 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="2" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" customWidth="1"/>
+    <col min="1" max="1" width="30.7090909090909" customWidth="1"/>
+    <col min="2" max="3" width="10.7090909090909" customWidth="1"/>
+    <col min="4" max="4" width="30.7090909090909" customWidth="1"/>
+    <col min="5" max="5" width="40.7090909090909" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" customHeight="1">
+    <row r="1" ht="18" customHeight="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="20" customHeight="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" ht="20" customHeight="1" spans="1:1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" ht="14.75" spans="2:3">
       <c r="B3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C3">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" ht="21.75" spans="1:5">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -764,7 +1454,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="16" customHeight="1">
+    <row r="5" ht="16" customHeight="1" spans="1:4">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -778,9 +1468,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16" customHeight="1">
+    <row r="6" ht="16" customHeight="1" spans="1:5">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
@@ -789,10 +1479,13 @@
         <v>1</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="16" customHeight="1">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" ht="16" customHeight="1" spans="1:4">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -803,12 +1496,12 @@
         <v>8</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="16" customHeight="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" ht="16" customHeight="1" spans="1:4">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -817,13 +1510,13 @@
         <v>1</v>
       </c>
       <c r="D8" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" ht="16" customHeight="1" spans="1:4">
+      <c r="A9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="16" customHeight="1">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
@@ -831,12 +1524,12 @@
         <v>1</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="16" customHeight="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" ht="16" customHeight="1" spans="1:4">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
@@ -845,12 +1538,12 @@
         <v>1</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="16" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" ht="16" customHeight="1" spans="1:4">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -859,12 +1552,12 @@
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="16" customHeight="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" ht="16" customHeight="1" spans="1:5">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
@@ -873,12 +1566,15 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="16" customHeight="1">
+        <v>25</v>
+      </c>
+      <c r="E12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" ht="16" customHeight="1" spans="1:4">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -887,12 +1583,12 @@
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="16" customHeight="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" ht="16" customHeight="1" spans="1:5">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
@@ -901,53 +1597,59 @@
         <v>16</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>30</v>
+        <v>35</v>
+      </c>
+      <c r="E14" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="2" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" customWidth="1"/>
+    <col min="1" max="1" width="30.7090909090909" customWidth="1"/>
+    <col min="2" max="3" width="10.7090909090909" customWidth="1"/>
+    <col min="4" max="4" width="30.7090909090909" customWidth="1"/>
+    <col min="5" max="5" width="40.7090909090909" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" customHeight="1">
+    <row r="1" ht="18" customHeight="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="20" customHeight="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" ht="20" customHeight="1" spans="1:1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" ht="14.75" spans="2:3">
       <c r="B3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C3">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" ht="21.75" spans="1:5">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -964,7 +1666,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="16" customHeight="1">
+    <row r="5" ht="16" customHeight="1" spans="1:4">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -978,9 +1680,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16" customHeight="1">
+    <row r="6" ht="16" customHeight="1" spans="1:4">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
@@ -989,12 +1691,12 @@
         <v>1</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="16" customHeight="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" ht="16" customHeight="1" spans="1:5">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
@@ -1003,26 +1705,29 @@
         <v>8</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="16" customHeight="1">
+        <v>38</v>
+      </c>
+      <c r="E7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" ht="16" customHeight="1" spans="1:4">
       <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" ht="16" customHeight="1" spans="1:5">
+      <c r="A9" t="s">
         <v>18</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="3">
-        <v>1</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="16" customHeight="1">
-      <c r="A9" t="s">
-        <v>17</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -1031,12 +1736,15 @@
         <v>1</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="16" customHeight="1">
+        <v>18</v>
+      </c>
+      <c r="E9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" ht="16" customHeight="1" spans="1:4">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -1045,12 +1753,12 @@
         <v>1</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="16" customHeight="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" ht="16" customHeight="1" spans="1:4">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -1059,12 +1767,12 @@
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="16" customHeight="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" ht="16" customHeight="1" spans="1:5">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
@@ -1073,10 +1781,14 @@
         <v>16</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>30</v>
+        <v>35</v>
+      </c>
+      <c r="E12" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: add some useful trait for `VerilogData` type
</commit_message>
<xml_diff>
--- a/src/excel/test/uart.xlsx
+++ b/src/excel/test/uart.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="42">
   <si>
     <t>Module Inst Name</t>
   </si>
@@ -63,45 +63,45 @@
     <t>rxd</t>
   </si>
   <si>
+    <t>s_axis_tready</t>
+  </si>
+  <si>
+    <t>s_axis_tvalid</t>
+  </si>
+  <si>
+    <t>txd</t>
+  </si>
+  <si>
+    <t>asdf</t>
+  </si>
+  <si>
+    <t>rx_busy</t>
+  </si>
+  <si>
+    <t>rx_frame_error</t>
+  </si>
+  <si>
+    <t>sadf</t>
+  </si>
+  <si>
+    <t>rx_overrun_error</t>
+  </si>
+  <si>
+    <t>tx_busy</t>
+  </si>
+  <si>
+    <t>test_clk</t>
+  </si>
+  <si>
+    <t>clk1</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
     <t>s_axis_tdata</t>
   </si>
   <si>
-    <t>s_axis_tready</t>
-  </si>
-  <si>
-    <t>s_axis_tvalid</t>
-  </si>
-  <si>
-    <t>txd</t>
-  </si>
-  <si>
-    <t>asdf</t>
-  </si>
-  <si>
-    <t>rx_busy</t>
-  </si>
-  <si>
-    <t>rx_frame_error</t>
-  </si>
-  <si>
-    <t>sadf</t>
-  </si>
-  <si>
-    <t>rx_overrun_error</t>
-  </si>
-  <si>
-    <t>tx_busy</t>
-  </si>
-  <si>
-    <t>test_clk</t>
-  </si>
-  <si>
-    <t>clk1</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
     <t>u_uart_rx</t>
   </si>
   <si>
@@ -135,16 +135,13 @@
     <t>u_uart_tx</t>
   </si>
   <si>
-    <t>s_axis_tdata[7:0]</t>
-  </si>
-  <si>
-    <t>反对敢死队风格Z</t>
-  </si>
-  <si>
     <t>告诉对方给</t>
   </si>
   <si>
     <t>fdgs</t>
+  </si>
+  <si>
+    <t>s_axis_tdata[14:0]</t>
   </si>
 </sst>
 </file>
@@ -640,10 +637,10 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C10" s="3">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="16" customHeight="1">
@@ -651,7 +648,7 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C11" s="3">
         <v>1</v>
@@ -662,24 +659,24 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C12" s="3">
         <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="16" customHeight="1">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="3">
         <v>1</v>
-      </c>
-      <c r="E13" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="16" customHeight="1">
@@ -692,19 +689,19 @@
       <c r="C14" s="3">
         <v>1</v>
       </c>
+      <c r="E14" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="15" spans="1:5" ht="16" customHeight="1">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="3">
         <v>1</v>
-      </c>
-      <c r="E15" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="16" customHeight="1">
@@ -723,24 +720,27 @@
         <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C17" s="3">
         <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="16" customHeight="1">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C18" s="3">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="16" customHeight="1">
@@ -748,13 +748,10 @@
         <v>27</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C19" s="3">
-        <v>1</v>
-      </c>
-      <c r="D19" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -828,7 +825,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16" customHeight="1">
@@ -901,7 +898,7 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="16" customHeight="1">
@@ -915,7 +912,7 @@
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E11" t="s">
         <v>33</v>
@@ -932,7 +929,7 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="16" customHeight="1">
@@ -1003,7 +1000,7 @@
         <v>29</v>
       </c>
       <c r="C3">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1053,38 +1050,38 @@
     </row>
     <row r="7" spans="1:5" ht="16" customHeight="1">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="3">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16" customHeight="1">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C8" s="3">
         <v>1</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="16" customHeight="1">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -1093,15 +1090,12 @@
         <v>1</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="16" customHeight="1">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -1109,39 +1103,39 @@
       <c r="C10" s="3">
         <v>1</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>18</v>
+      <c r="D10" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="16" customHeight="1">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C11" s="3">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>24</v>
+        <v>16</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="16" customHeight="1">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="3">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: fix bug of excel writer macro
</commit_message>
<xml_diff>
--- a/src/excel/test/uart.xlsx
+++ b/src/excel/test/uart.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="40">
   <si>
     <t>Module Inst Name</t>
   </si>
@@ -45,24 +45,39 @@
     <t>input</t>
   </si>
   <si>
+    <t>m_axis_tdata</t>
+  </si>
+  <si>
+    <t>output</t>
+  </si>
+  <si>
+    <t>afd</t>
+  </si>
+  <si>
+    <t>test1</t>
+  </si>
+  <si>
     <t>m_axis_tready</t>
   </si>
   <si>
     <t>m_axis_tvalid</t>
   </si>
   <si>
-    <t>output</t>
-  </si>
-  <si>
     <t>prescale</t>
   </si>
   <si>
     <t>rst</t>
   </si>
   <si>
+    <t>fadsf</t>
+  </si>
+  <si>
     <t>rxd</t>
   </si>
   <si>
+    <t>s_axis_tdata</t>
+  </si>
+  <si>
     <t>s_axis_tready</t>
   </si>
   <si>
@@ -72,7 +87,7 @@
     <t>txd</t>
   </si>
   <si>
-    <t>asdf</t>
+    <t>test1, test2</t>
   </si>
   <si>
     <t>rx_busy</t>
@@ -81,34 +96,25 @@
     <t>rx_frame_error</t>
   </si>
   <si>
-    <t>sadf</t>
-  </si>
-  <si>
     <t>rx_overrun_error</t>
   </si>
   <si>
     <t>tx_busy</t>
   </si>
   <si>
-    <t>test_clk</t>
-  </si>
-  <si>
-    <t>clk1</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>s_axis_tdata</t>
-  </si>
-  <si>
     <t>u_uart_rx</t>
   </si>
   <si>
     <t>DATA_WIDTH</t>
   </si>
   <si>
-    <t>asdfasd</t>
+    <t>test2</t>
+  </si>
+  <si>
+    <t>m_axis_tdata[7:0]</t>
+  </si>
+  <si>
+    <t>fgs</t>
   </si>
   <si>
     <t>busy</t>
@@ -117,31 +123,19 @@
     <t>overrun_error</t>
   </si>
   <si>
-    <t>fdasf</t>
-  </si>
-  <si>
     <t>frame_error</t>
   </si>
   <si>
     <t>prescale[15:0]</t>
   </si>
   <si>
-    <t>asf</t>
-  </si>
-  <si>
-    <t>m_axis_tdata</t>
-  </si>
-  <si>
     <t>u_uart_tx</t>
   </si>
   <si>
-    <t>告诉对方给</t>
-  </si>
-  <si>
-    <t>fdgs</t>
-  </si>
-  <si>
-    <t>s_axis_tdata[14:0]</t>
+    <t>s_axis_tdata[7:0]</t>
+  </si>
+  <si>
+    <t>sdfg</t>
   </si>
 </sst>
 </file>
@@ -524,7 +518,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
@@ -537,19 +531,20 @@
     <col min="2" max="3" width="10.7109375" customWidth="1"/>
     <col min="4" max="4" width="30.7109375" customWidth="1"/>
     <col min="5" max="5" width="40.7109375" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" customHeight="1">
+    <row r="1" spans="1:6" ht="18" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="20" customHeight="1">
+    <row r="2" spans="1:6" ht="20" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -565,8 +560,9 @@
       <c r="E3" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="16" customHeight="1">
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" ht="16" customHeight="1">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -577,53 +573,59 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="16" customHeight="1">
+    <row r="5" spans="1:6" ht="16" customHeight="1">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C5" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="16" customHeight="1">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16" customHeight="1">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C6" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16" customHeight="1">
+    <row r="7" spans="1:6" ht="16" customHeight="1">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16" customHeight="1">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="3">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="16" customHeight="1">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="16" customHeight="1">
+    <row r="9" spans="1:6" ht="16" customHeight="1">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
@@ -631,127 +633,110 @@
       <c r="C9" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="16" customHeight="1">
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16" customHeight="1">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C10" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="16" customHeight="1">
+    <row r="11" spans="1:6" ht="16" customHeight="1">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="16" customHeight="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16" customHeight="1">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="3">
         <v>1</v>
       </c>
-      <c r="E12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="16" customHeight="1">
+    </row>
+    <row r="13" spans="1:6" ht="16" customHeight="1">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C13" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="16" customHeight="1">
+    <row r="14" spans="1:6" ht="16" customHeight="1">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C14" s="3">
         <v>1</v>
       </c>
-      <c r="E14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="16" customHeight="1">
+      <c r="F14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="16" customHeight="1">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C15" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="16" customHeight="1">
+    <row r="16" spans="1:6" ht="16" customHeight="1">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C16" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="16" customHeight="1">
+    <row r="17" spans="1:3" ht="16" customHeight="1">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C17" s="3">
         <v>1</v>
       </c>
-      <c r="D17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="16" customHeight="1">
+    </row>
+    <row r="18" spans="1:3" ht="16" customHeight="1">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C18" s="3">
         <v>1</v>
-      </c>
-      <c r="D18" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="16" customHeight="1">
-      <c r="A19" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="3">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -761,7 +746,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
@@ -774,9 +759,10 @@
     <col min="2" max="3" width="10.7109375" customWidth="1"/>
     <col min="4" max="4" width="30.7109375" customWidth="1"/>
     <col min="5" max="5" width="40.7109375" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" customHeight="1">
+    <row r="1" spans="1:6" ht="18" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -784,20 +770,20 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="20" customHeight="1">
+    <row r="2" spans="1:6" ht="20" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="B3" t="s">
         <v>29</v>
       </c>
       <c r="C3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -813,8 +799,11 @@
       <c r="E4" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="16" customHeight="1">
+      <c r="F4" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="16" customHeight="1">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -824,140 +813,137 @@
       <c r="C5" s="3">
         <v>1</v>
       </c>
-      <c r="D5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="16" customHeight="1">
+      <c r="D5" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16" customHeight="1">
       <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16" customHeight="1">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="3">
+        <v>8</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16" customHeight="1">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16" customHeight="1">
+      <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="3">
-        <v>1</v>
-      </c>
-      <c r="D6" s="4" t="s">
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="16" customHeight="1">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="3">
-        <v>1</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="16" customHeight="1">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="3">
-        <v>1</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="16" customHeight="1">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="3">
-        <v>1</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="16" customHeight="1">
+    </row>
+    <row r="10" spans="1:6" ht="16" customHeight="1">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C10" s="3">
         <v>1</v>
       </c>
-      <c r="D10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="16" customHeight="1">
+      <c r="D10" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16" customHeight="1">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="3">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="16" customHeight="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16" customHeight="1">
       <c r="A12" t="s">
         <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="3">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="16" customHeight="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="16" customHeight="1">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C13" s="3">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="16" customHeight="1">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="3">
         <v>16</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="D14" s="4" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="16" customHeight="1">
-      <c r="A14" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="3">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -967,7 +953,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
@@ -980,30 +966,31 @@
     <col min="2" max="3" width="10.7109375" customWidth="1"/>
     <col min="4" max="4" width="30.7109375" customWidth="1"/>
     <col min="5" max="5" width="40.7109375" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" customHeight="1">
+    <row r="1" spans="1:6" ht="18" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="20" customHeight="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="20" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="B3" t="s">
         <v>29</v>
       </c>
       <c r="C3">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -1019,8 +1006,9 @@
       <c r="E4" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="16" customHeight="1">
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" ht="16" customHeight="1">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1034,9 +1022,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16" customHeight="1">
+    <row r="6" spans="1:6" ht="16" customHeight="1">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
@@ -1045,97 +1033,94 @@
         <v>1</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="16" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16" customHeight="1">
       <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="3">
+        <v>8</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16" customHeight="1">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16" customHeight="1">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16" customHeight="1">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16" customHeight="1">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16" customHeight="1">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="3">
         <v>16</v>
       </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="3">
-        <v>1</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="16" customHeight="1">
-      <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="3">
-        <v>1</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="16" customHeight="1">
-      <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="3">
-        <v>1</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="16" customHeight="1">
-      <c r="A10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="3">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="16" customHeight="1">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="3">
-        <v>16</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="16" customHeight="1">
-      <c r="A12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="3">
-        <v>15</v>
-      </c>
       <c r="D12" s="4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: fix bug of not update wire which connected to the port which update its width by parameter
</commit_message>
<xml_diff>
--- a/src/excel/test/uart.xlsx
+++ b/src/excel/test/uart.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="36">
   <si>
     <t>Module Inst Name</t>
   </si>
@@ -45,76 +45,58 @@
     <t>input</t>
   </si>
   <si>
+    <t>m_axis_tready</t>
+  </si>
+  <si>
+    <t>m_axis_tvalid</t>
+  </si>
+  <si>
+    <t>output</t>
+  </si>
+  <si>
+    <t>prescale</t>
+  </si>
+  <si>
+    <t>rst</t>
+  </si>
+  <si>
+    <t>rxd</t>
+  </si>
+  <si>
+    <t>s_axis_tdata</t>
+  </si>
+  <si>
+    <t>s_axis_tready</t>
+  </si>
+  <si>
+    <t>s_axis_tvalid</t>
+  </si>
+  <si>
+    <t>txd</t>
+  </si>
+  <si>
+    <t>rx_busy</t>
+  </si>
+  <si>
+    <t>rx_frame_error</t>
+  </si>
+  <si>
+    <t>rx_overrun_error</t>
+  </si>
+  <si>
+    <t>tx_busy</t>
+  </si>
+  <si>
     <t>m_axis_tdata</t>
   </si>
   <si>
-    <t>output</t>
-  </si>
-  <si>
-    <t>afd</t>
-  </si>
-  <si>
-    <t>test1</t>
-  </si>
-  <si>
-    <t>m_axis_tready</t>
-  </si>
-  <si>
-    <t>m_axis_tvalid</t>
-  </si>
-  <si>
-    <t>prescale</t>
-  </si>
-  <si>
-    <t>rst</t>
-  </si>
-  <si>
-    <t>fadsf</t>
-  </si>
-  <si>
-    <t>rxd</t>
-  </si>
-  <si>
-    <t>s_axis_tdata</t>
-  </si>
-  <si>
-    <t>s_axis_tready</t>
-  </si>
-  <si>
-    <t>s_axis_tvalid</t>
-  </si>
-  <si>
-    <t>txd</t>
-  </si>
-  <si>
-    <t>test1, test2</t>
-  </si>
-  <si>
-    <t>rx_busy</t>
-  </si>
-  <si>
-    <t>rx_frame_error</t>
-  </si>
-  <si>
-    <t>rx_overrun_error</t>
-  </si>
-  <si>
-    <t>tx_busy</t>
-  </si>
-  <si>
     <t>u_uart_rx</t>
   </si>
   <si>
     <t>DATA_WIDTH</t>
   </si>
   <si>
-    <t>test2</t>
-  </si>
-  <si>
-    <t>m_axis_tdata[7:0]</t>
-  </si>
-  <si>
-    <t>fgs</t>
+    <t>sdfa</t>
   </si>
   <si>
     <t>busy</t>
@@ -129,13 +111,19 @@
     <t>prescale[15:0]</t>
   </si>
   <si>
+    <t>m_axis_tdata[21:0]</t>
+  </si>
+  <si>
     <t>u_uart_tx</t>
   </si>
   <si>
     <t>s_axis_tdata[7:0]</t>
   </si>
   <si>
-    <t>sdfg</t>
+    <t>daf</t>
+  </si>
+  <si>
+    <t>dsaf</t>
   </si>
 </sst>
 </file>
@@ -212,16 +200,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -569,7 +554,7 @@
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4">
         <v>1</v>
       </c>
     </row>
@@ -578,165 +563,153 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="3">
-        <v>8</v>
-      </c>
-      <c r="E5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16" customHeight="1">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="3">
+        <v>11</v>
+      </c>
+      <c r="C6">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16" customHeight="1">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="3">
-        <v>1</v>
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16" customHeight="1">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="3">
-        <v>16</v>
+      <c r="C8">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" customHeight="1">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="3">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
-        <v>17</v>
+      <c r="C9">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16" customHeight="1">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="3">
-        <v>1</v>
+      <c r="C10">
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16" customHeight="1">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="3">
-        <v>8</v>
+        <v>11</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16" customHeight="1">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="3">
+        <v>8</v>
+      </c>
+      <c r="C12">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="16" customHeight="1">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="3">
+        <v>11</v>
+      </c>
+      <c r="C13">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="16" customHeight="1">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="3">
-        <v>1</v>
-      </c>
-      <c r="F14" t="s">
-        <v>23</v>
+        <v>11</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="16" customHeight="1">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="3">
+        <v>11</v>
+      </c>
+      <c r="C15">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="16" customHeight="1">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="3">
+        <v>11</v>
+      </c>
+      <c r="C16">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="16" customHeight="1">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="3">
+        <v>11</v>
+      </c>
+      <c r="C17">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="16" customHeight="1">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="3">
-        <v>1</v>
+        <v>11</v>
+      </c>
+      <c r="C18">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -767,7 +740,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="20" customHeight="1">
@@ -777,10 +750,10 @@
     </row>
     <row r="3" spans="1:6">
       <c r="B3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C3">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -799,9 +772,7 @@
       <c r="E4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>30</v>
-      </c>
+      <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" ht="16" customHeight="1">
       <c r="A5" t="s">
@@ -810,140 +781,140 @@
       <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="3">
-        <v>1</v>
-      </c>
-      <c r="D5" s="4" t="s">
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16" customHeight="1">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="3">
-        <v>1</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>16</v>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16" customHeight="1">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="C7" s="3">
-        <v>8</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16" customHeight="1">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="3">
-        <v>1</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" customHeight="1">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="3">
-        <v>1</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>13</v>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16" customHeight="1">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="3">
-        <v>1</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16" customHeight="1">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="3">
+        <v>11</v>
+      </c>
+      <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16" customHeight="1">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="3">
+        <v>11</v>
+      </c>
+      <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="16" customHeight="1">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="3">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
-        <v>25</v>
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>16</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="16" customHeight="1">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="3">
-        <v>16</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>36</v>
+        <v>11</v>
+      </c>
+      <c r="C14">
+        <v>22</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -974,7 +945,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="20" customHeight="1">
@@ -984,7 +955,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="B3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C3">
         <v>8</v>
@@ -1015,112 +986,115 @@
       <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="3">
-        <v>1</v>
-      </c>
-      <c r="D5" s="4" t="s">
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16" customHeight="1">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="3">
-        <v>1</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>16</v>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16" customHeight="1">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="3">
-        <v>8</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>38</v>
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="E7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16" customHeight="1">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="3">
-        <v>1</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>21</v>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" customHeight="1">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="3">
-        <v>1</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>20</v>
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16" customHeight="1">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="3">
-        <v>1</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>22</v>
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16" customHeight="1">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="3">
+        <v>11</v>
+      </c>
+      <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>22</v>
+      </c>
+      <c r="E11" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16" customHeight="1">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12">
         <v>16</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>36</v>
+      <c r="D12" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add name verify
</commit_message>
<xml_diff>
--- a/src/excel/test/uart.xlsx
+++ b/src/excel/test/uart.xlsx
@@ -1,22 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView windowWidth="30450" windowHeight="14460"/>
   </bookViews>
   <sheets>
     <sheet name="uart" sheetId="1" r:id="rId1"/>
     <sheet name="uart_rx" sheetId="2" r:id="rId2"/>
     <sheet name="uart_tx" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="36">
   <si>
     <t>Module Inst Name</t>
   </si>
@@ -54,116 +67,266 @@
     <t>output</t>
   </si>
   <si>
+    <t>rst</t>
+  </si>
+  <si>
+    <t>rxd</t>
+  </si>
+  <si>
+    <t>s_axis_tdata</t>
+  </si>
+  <si>
+    <t>s_axis_tready</t>
+  </si>
+  <si>
+    <t>txd</t>
+  </si>
+  <si>
+    <t>rx_frame_error</t>
+  </si>
+  <si>
+    <t>tx_busy</t>
+  </si>
+  <si>
+    <t>testdata</t>
+  </si>
+  <si>
+    <t>m_axis_tdata</t>
+  </si>
+  <si>
+    <t>u_uart_rx</t>
+  </si>
+  <si>
+    <t>DATA_WIDTH</t>
+  </si>
+  <si>
+    <t>test1</t>
+  </si>
+  <si>
+    <t>busy</t>
+  </si>
+  <si>
+    <t>rx_busy</t>
+  </si>
+  <si>
+    <t>overrun_error</t>
+  </si>
+  <si>
+    <t>rx_overrun_error</t>
+  </si>
+  <si>
+    <t>frame_error</t>
+  </si>
+  <si>
     <t>prescale</t>
   </si>
   <si>
-    <t>rst</t>
-  </si>
-  <si>
-    <t>rxd</t>
-  </si>
-  <si>
-    <t>s_axis_tdata</t>
-  </si>
-  <si>
-    <t>s_axis_tready</t>
+    <t>prescale[15:0]</t>
+  </si>
+  <si>
+    <t>m_axis_tdata[15:0]</t>
+  </si>
+  <si>
+    <t>u_uart_tx</t>
+  </si>
+  <si>
+    <t>s_axis_tdata[7:0]</t>
   </si>
   <si>
     <t>s_axis_tvalid</t>
   </si>
   <si>
-    <t>txd</t>
-  </si>
-  <si>
-    <t>rx_busy</t>
-  </si>
-  <si>
-    <t>rx_frame_error</t>
-  </si>
-  <si>
-    <t>rx_overrun_error</t>
-  </si>
-  <si>
-    <t>tx_busy</t>
-  </si>
-  <si>
-    <t>m_axis_tdata</t>
-  </si>
-  <si>
-    <t>u_uart_rx</t>
-  </si>
-  <si>
-    <t>DATA_WIDTH</t>
-  </si>
-  <si>
-    <t>sdfa</t>
-  </si>
-  <si>
-    <t>busy</t>
-  </si>
-  <si>
-    <t>overrun_error</t>
-  </si>
-  <si>
-    <t>frame_error</t>
-  </si>
-  <si>
-    <t>prescale[15:0]</t>
-  </si>
-  <si>
-    <t>m_axis_tdata[21:0]</t>
-  </si>
-  <si>
-    <t>u_uart_tx</t>
-  </si>
-  <si>
-    <t>s_axis_tdata[7:0]</t>
-  </si>
-  <si>
-    <t>daf</t>
-  </si>
-  <si>
-    <t>dsaf</t>
+    <t>test2, test1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -176,8 +339,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -196,9 +545,251 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -210,11 +801,63 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -497,39 +1140,40 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="2" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="30.7083333333333" customWidth="1"/>
+    <col min="2" max="3" width="10.7083333333333" customWidth="1"/>
+    <col min="4" max="4" width="30.7083333333333" customWidth="1"/>
+    <col min="5" max="5" width="40.7083333333333" customWidth="1"/>
+    <col min="6" max="6" width="20.7083333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" customHeight="1">
+    <row r="1" ht="18" customHeight="1" spans="1:1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="20" customHeight="1">
+    <row r="2" ht="20" customHeight="1" spans="1:1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" ht="21" spans="1:6">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -547,7 +1191,7 @@
       </c>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" ht="16" customHeight="1">
+    <row r="4" ht="16" customHeight="1" spans="1:3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -558,7 +1202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16" customHeight="1">
+    <row r="5" ht="16" customHeight="1" spans="1:3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -569,7 +1213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16" customHeight="1">
+    <row r="6" ht="16" customHeight="1" spans="1:3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -580,7 +1224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16" customHeight="1">
+    <row r="7" ht="16" customHeight="1" spans="1:3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -588,10 +1232,10 @@
         <v>8</v>
       </c>
       <c r="C7">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="16" customHeight="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" ht="16" customHeight="1" spans="1:3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -602,7 +1246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="16" customHeight="1">
+    <row r="9" ht="16" customHeight="1" spans="1:3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -610,21 +1254,21 @@
         <v>8</v>
       </c>
       <c r="C9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="16" customHeight="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" ht="16" customHeight="1" spans="1:3">
       <c r="A10" t="s">
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="16" customHeight="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" ht="16" customHeight="1" spans="1:3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -635,18 +1279,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="16" customHeight="1">
+    <row r="12" ht="16" customHeight="1" spans="1:3">
       <c r="A12" t="s">
         <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="16" customHeight="1">
+    <row r="13" ht="16" customHeight="1" spans="1:3">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -657,7 +1301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="16" customHeight="1">
+    <row r="14" ht="16" customHeight="1" spans="1:4">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -665,98 +1309,60 @@
         <v>11</v>
       </c>
       <c r="C14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="16" customHeight="1">
-      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" t="s">
         <v>20</v>
-      </c>
-      <c r="B15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="16" customHeight="1">
-      <c r="A16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="16" customHeight="1">
-      <c r="A17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="16" customHeight="1">
-      <c r="A18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="2" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="30.7083333333333" customWidth="1"/>
+    <col min="2" max="3" width="10.7083333333333" customWidth="1"/>
+    <col min="4" max="4" width="30.7083333333333" customWidth="1"/>
+    <col min="5" max="5" width="40.7083333333333" customWidth="1"/>
+    <col min="6" max="6" width="20.7083333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" customHeight="1">
+    <row r="1" ht="18" customHeight="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="20" customHeight="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" ht="20" customHeight="1" spans="1:1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" ht="14.25" spans="2:3">
       <c r="B3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C3">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" ht="21" spans="1:6">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -772,9 +1378,11 @@
       <c r="E4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" ht="16" customHeight="1">
+      <c r="F4" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" ht="16" customHeight="1" spans="1:4">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -788,9 +1396,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16" customHeight="1">
+    <row r="6" ht="16" customHeight="1" spans="1:4">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
@@ -799,10 +1407,10 @@
         <v>1</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="16" customHeight="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" ht="16" customHeight="1" spans="1:4">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -816,7 +1424,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16" customHeight="1">
+    <row r="8" ht="16" customHeight="1" spans="1:4">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -829,13 +1437,10 @@
       <c r="D8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="16" customHeight="1">
+    </row>
+    <row r="9" ht="16" customHeight="1" spans="1:4">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
@@ -844,12 +1449,12 @@
         <v>1</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="16" customHeight="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" ht="16" customHeight="1" spans="1:4">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -858,12 +1463,12 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="16" customHeight="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" ht="16" customHeight="1" spans="1:4">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -872,12 +1477,12 @@
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="16" customHeight="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" ht="16" customHeight="1" spans="1:4">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
@@ -886,12 +1491,12 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="16" customHeight="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" ht="16" customHeight="1" spans="1:4">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="B13" t="s">
         <v>8</v>
@@ -903,15 +1508,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="16" customHeight="1">
+    <row r="14" ht="16" customHeight="1" spans="1:4">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
       </c>
       <c r="C14">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>31</v>
@@ -919,28 +1524,31 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="2" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="30.7083333333333" customWidth="1"/>
+    <col min="2" max="3" width="10.7083333333333" customWidth="1"/>
+    <col min="4" max="4" width="30.7083333333333" customWidth="1"/>
+    <col min="5" max="5" width="40.7083333333333" customWidth="1"/>
+    <col min="6" max="6" width="20.7083333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" customHeight="1">
+    <row r="1" ht="18" customHeight="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -948,20 +1556,20 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="20" customHeight="1">
+    <row r="2" ht="20" customHeight="1" spans="1:1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" ht="14.25" spans="2:3">
       <c r="B3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C3">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" ht="21" spans="1:6">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -979,7 +1587,7 @@
       </c>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" ht="16" customHeight="1">
+    <row r="5" ht="16" customHeight="1" spans="1:4">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -993,9 +1601,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16" customHeight="1">
+    <row r="6" ht="16" customHeight="1" spans="1:4">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
@@ -1003,13 +1611,13 @@
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="16" customHeight="1">
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" ht="16" customHeight="1" spans="1:4">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
@@ -1020,13 +1628,10 @@
       <c r="D7" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E7" t="s">
+    </row>
+    <row r="8" ht="16" customHeight="1" spans="1:6">
+      <c r="A8" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="16" customHeight="1">
-      <c r="A8" t="s">
-        <v>17</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -1034,13 +1639,16 @@
       <c r="C8">
         <v>1</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="16" customHeight="1">
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" ht="16" customHeight="1" spans="1:4">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -1049,12 +1657,12 @@
         <v>1</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" ht="16" customHeight="1" spans="1:4">
+      <c r="A10" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="16" customHeight="1">
-      <c r="A10" t="s">
-        <v>18</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -1063,12 +1671,12 @@
         <v>1</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="16" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" ht="16" customHeight="1" spans="1:6">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -1077,18 +1685,18 @@
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="16" customHeight="1">
+    <row r="12" ht="16" customHeight="1" spans="1:4">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C12">
         <v>16</v>
@@ -1099,5 +1707,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: add enter delimiter support
</commit_message>
<xml_diff>
--- a/src/excel/test/uart.xlsx
+++ b/src/excel/test/uart.xlsx
@@ -1,22 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView windowWidth="30450" windowHeight="14460" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="uart" sheetId="1" r:id="rId1"/>
     <sheet name="uart_rx" sheetId="2" r:id="rId2"/>
     <sheet name="uart_tx" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="38">
   <si>
     <t>Module Inst Name</t>
   </si>
@@ -108,22 +121,40 @@
     <t>frame_error</t>
   </si>
   <si>
+    <t>test1
+test2
+test3
+test4
+test5
+test6
+test7
+test8
+test9
+test10
+test11
+test12
+test13
+test14
+test15
+test16</t>
+  </si>
+  <si>
+    <t>m_axis_tdata[5:0]</t>
+  </si>
+  <si>
+    <t>u_uart_tx</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>s_axis_tvalid</t>
+  </si>
+  <si>
+    <t>test2, test1</t>
+  </si>
+  <si>
     <t>prescale[15:0]</t>
-  </si>
-  <si>
-    <t>m_axis_tdata[5:0]</t>
-  </si>
-  <si>
-    <t>u_uart_tx</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>s_axis_tvalid</t>
-  </si>
-  <si>
-    <t>test2, test1</t>
   </si>
   <si>
     <t>s_axis_tdata[7:0]</t>
@@ -132,41 +163,198 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -179,8 +367,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -199,11 +573,253 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -212,12 +828,67 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -500,39 +1171,40 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="2" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="30.7083333333333" customWidth="1"/>
+    <col min="2" max="3" width="10.7083333333333" customWidth="1"/>
+    <col min="4" max="4" width="30.7083333333333" customWidth="1"/>
+    <col min="5" max="5" width="40.7083333333333" customWidth="1"/>
+    <col min="6" max="6" width="20.7083333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" customHeight="1">
+    <row r="1" ht="18" customHeight="1" spans="1:1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="20" customHeight="1">
+    <row r="2" ht="20" customHeight="1" spans="1:1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" ht="21" spans="1:6">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -550,7 +1222,7 @@
       </c>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" ht="16" customHeight="1">
+    <row r="4" ht="16" customHeight="1" spans="1:3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -561,7 +1233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16" customHeight="1">
+    <row r="5" ht="16" customHeight="1" spans="1:3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -572,7 +1244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16" customHeight="1">
+    <row r="6" ht="16" customHeight="1" spans="1:3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -583,7 +1255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16" customHeight="1">
+    <row r="7" ht="16" customHeight="1" spans="1:3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -594,7 +1266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16" customHeight="1">
+    <row r="8" ht="16" customHeight="1" spans="1:3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -605,7 +1277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="16" customHeight="1">
+    <row r="9" ht="16" customHeight="1" spans="1:3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -616,7 +1288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16" customHeight="1">
+    <row r="10" ht="16" customHeight="1" spans="1:3">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -627,7 +1299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16" customHeight="1">
+    <row r="11" ht="16" customHeight="1" spans="1:3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -638,7 +1310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="16" customHeight="1">
+    <row r="12" ht="16" customHeight="1" spans="1:3">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -649,7 +1321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="16" customHeight="1">
+    <row r="13" ht="16" customHeight="1" spans="1:3">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -660,7 +1332,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="16" customHeight="1">
+    <row r="14" ht="16" customHeight="1" spans="1:3">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -671,7 +1343,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="16" customHeight="1">
+    <row r="15" ht="16" customHeight="1" spans="1:3">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -684,28 +1356,31 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="2" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="30.7083333333333" customWidth="1"/>
+    <col min="2" max="3" width="10.7083333333333" customWidth="1"/>
+    <col min="4" max="4" width="30.7083333333333" customWidth="1"/>
+    <col min="5" max="5" width="40.7083333333333" customWidth="1"/>
+    <col min="6" max="6" width="20.7083333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" customHeight="1">
+    <row r="1" ht="18" customHeight="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -713,12 +1388,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="20" customHeight="1">
+    <row r="2" ht="20" customHeight="1" spans="1:1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" ht="14.25" spans="2:3">
       <c r="B3" t="s">
         <v>22</v>
       </c>
@@ -726,7 +1401,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" ht="21" spans="1:6">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -746,7 +1421,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16" customHeight="1">
+    <row r="5" ht="16" customHeight="1" spans="1:4">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -760,7 +1435,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16" customHeight="1">
+    <row r="6" ht="16" customHeight="1" spans="1:4">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -774,7 +1449,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16" customHeight="1">
+    <row r="7" ht="16" customHeight="1" spans="1:4">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -788,7 +1463,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16" customHeight="1">
+    <row r="8" ht="16" customHeight="1" spans="1:4">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -802,7 +1477,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="16" customHeight="1">
+    <row r="9" ht="16" customHeight="1" spans="1:4">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -816,7 +1491,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16" customHeight="1">
+    <row r="10" ht="16" customHeight="1" spans="1:4">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -830,7 +1505,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16" customHeight="1">
+    <row r="11" ht="16" customHeight="1" spans="1:4">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -844,7 +1519,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="16" customHeight="1">
+    <row r="12" ht="16" customHeight="1" spans="1:4">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -858,7 +1533,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="16" customHeight="1">
+    <row r="13" ht="216" spans="1:4">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -868,11 +1543,11 @@
       <c r="C13">
         <v>16</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="16" customHeight="1">
+    <row r="14" ht="16" customHeight="1" spans="1:4">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -888,28 +1563,31 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="2" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="30.7083333333333" customWidth="1"/>
+    <col min="2" max="3" width="10.7083333333333" customWidth="1"/>
+    <col min="4" max="4" width="30.7083333333333" customWidth="1"/>
+    <col min="5" max="5" width="40.7083333333333" customWidth="1"/>
+    <col min="6" max="6" width="20.7083333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" customHeight="1">
+    <row r="1" ht="18" customHeight="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -917,12 +1595,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="20" customHeight="1">
+    <row r="2" ht="20" customHeight="1" spans="1:1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" ht="14.25" spans="2:3">
       <c r="B3" t="s">
         <v>22</v>
       </c>
@@ -930,7 +1608,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" ht="21" spans="1:6">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -948,7 +1626,7 @@
       </c>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" ht="16" customHeight="1">
+    <row r="5" ht="16" customHeight="1" spans="1:4">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -962,7 +1640,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16" customHeight="1">
+    <row r="6" ht="16" customHeight="1" spans="1:4">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -976,7 +1654,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16" customHeight="1">
+    <row r="7" ht="16" customHeight="1" spans="1:6">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -993,7 +1671,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16" customHeight="1">
+    <row r="8" ht="16" customHeight="1" spans="1:4">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1007,7 +1685,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="16" customHeight="1">
+    <row r="9" ht="16" customHeight="1" spans="1:4">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1021,7 +1699,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16" customHeight="1">
+    <row r="10" ht="16" customHeight="1" spans="1:6">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -1038,7 +1716,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16" customHeight="1">
+    <row r="11" ht="16" customHeight="1" spans="1:4">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1049,10 +1727,10 @@
         <v>16</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="16" customHeight="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" ht="16" customHeight="1" spans="1:4">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -1063,10 +1741,11 @@
         <v>8</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>